<commit_message>
Updated excel files with words
</commit_message>
<xml_diff>
--- a/wortschatz.xlsx
+++ b/wortschatz.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="892">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="1061">
   <si>
     <t xml:space="preserve">Wort</t>
   </si>
@@ -2696,6 +2696,545 @@
   </si>
   <si>
     <t xml:space="preserve">anaesthesia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Abfall, Abfälle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">garbage, trash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Bauer, Bauern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the farmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Bäuerin, Bäuerinnen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the farmer (fem)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Biene, Bienen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the bee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Dreck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the dirt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Einnahme, -n (≠die Ausgabe, -n)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Experte,-n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the expert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das Feuer, -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the fire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Forschung,-en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the scientific research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Frucht, -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the fruit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das Gift, -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the poison, venom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das Gras, Gräser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Bauernhof, Bauernhöfe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das Insekt, Insekten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the insect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das Klima, Klimata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the climate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Kuh, Kühe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the cow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das Labor, -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the laboratory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Mücke, -n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the mosquito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Produktion, -en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das Rind, -er</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the beef</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Steckdose, -n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the wallsocket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Stecker, -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the plug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Umwelt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Umweltverschmutzung, -en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the pollution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das Waschmittel, -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the washing powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Wissenschaft, -en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the science</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Wissenschaftler, -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the scientist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Zweifel, -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the doubt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atmen- er atmet-atmete-hat geatmet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to breath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(etwas von Dat) aufheben-er hebt auf- hob auf- hat aufgehoben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to pick smth (from somewhere)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etw (von etw/jdm) behaupten-er behauptet-behauptete-hat behauptet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to claim smth about smbd/smth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heizen-er heizt-heizte-hat geheizt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to heat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">produzieren-er produziert-produzierte-hat produziert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to produce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schützen (vor etw/jmd)-er schützt-schützte-hat geschützt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to protect (from smth/sbd)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weltweit (= global)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">worldwide, global</t>
+  </si>
+  <si>
+    <t xml:space="preserve">grundsätzlich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fundamental</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ökologisch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ecological</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schädlich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">harmful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sinnlos (≠sinnvoll)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">senseless</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wertvoll (≠wertlos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valuable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Luft, Lüfte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the air</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Ware, -n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the article, product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ernten-er erntet-erntete-hat geerntet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to harvest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waschen-er wäscht-wusch-hat gewaschen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to wash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mischen-er mischt-mischte-hat gemischt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to mix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Kenntnis, Kenntnisse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the knowledge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Davon habe ich keine Kenntniss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Karriere, Karrieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the carreer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Lebenslauf, Lebensläufe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the cv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Leitung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the guidance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Mietpreis, Mietpreise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the rent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das Anschreiben, -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the cover letter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sich bewerben um + Akk - er bewirbt sich – bewarb sich – hat sich beworben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Man muss ein Anscreiben screiben, wenn man sich um eine Stelle bewirbt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Anzeige, -n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the advertisment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Bedingung, -en </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the condition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notwendig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">necessary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Bereich, Bereiche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">realm, section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beherrschen-er beherrscht-beherrschte- hat beherrscht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to master smth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sie beherrscht ihr Handwerk. Ein Instrument beherrschen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beherrschen sich -er beherrscht sich-beherrschte sich- hat sich beherrscht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to control oneself</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beherrshen Sie sich!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">beschäftigen sich mit -er beschäftigt-beschäftigte sich-hat sich beschäftigt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">to busy oneself with</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erwin beschäftigt sich gerade mit der Abrechnung.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">auswendig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">by heart, from memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etwas auswendig lernen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schon immer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all along</t>
+  </si>
+  <si>
+    <t xml:space="preserve">erfolgreich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">successful</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ich möchte eine erfolgreiche Karriere haben.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Wirklichkeit, -en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tatsächlich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">actually</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">häufig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">common</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Griff, -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the grasp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hast du alles im Griff?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vor allem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">first of all, above all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Gebrauch, Gebräuche (=die Benutzung, die Verwendung)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the useage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ziemlich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fairly, quite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obst bei Rewe sind ziemlich gunstig.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">die Schwäche, -n (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">≠ die Stärke)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">the weakness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anzeichen von Schwäche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Stimmung, -en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tätig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Tätigkeit, -en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the activity</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">teilzeit arbeiten (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">≠ vollzeit)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Part-time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">das Unternehmen, - (die Firma, der Betrieb)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">der Wünsch, -e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selbständig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">independent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">momentan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at the moment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Anstellung, -en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the employment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">die Bewerbung, -en</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eine Bewerbung für eine Stelle einreichen</t>
   </si>
 </sst>
 </file>
@@ -2706,7 +3245,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -2726,6 +3265,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2776,7 +3321,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2786,6 +3331,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2806,16 +3355,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C450"/>
+  <dimension ref="A1:D531"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A416" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C451" activeCellId="0" sqref="C451"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A493" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A532" activeCellId="0" sqref="A532"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="67.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="63.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7766,6 +8316,930 @@
       </c>
       <c r="C450" s="0" t="s">
         <v>891</v>
+      </c>
+    </row>
+    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A451" s="0" t="s">
+        <v>892</v>
+      </c>
+      <c r="B451" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C451" s="0" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A452" s="0" t="s">
+        <v>894</v>
+      </c>
+      <c r="B452" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C452" s="0" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A453" s="0" t="s">
+        <v>896</v>
+      </c>
+      <c r="B453" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C453" s="0" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A454" s="0" t="s">
+        <v>898</v>
+      </c>
+      <c r="B454" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C454" s="0" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A455" s="0" t="s">
+        <v>900</v>
+      </c>
+      <c r="B455" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C455" s="0" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A456" s="0" t="s">
+        <v>902</v>
+      </c>
+      <c r="B456" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C456" s="0" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A457" s="0" t="s">
+        <v>904</v>
+      </c>
+      <c r="B457" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C457" s="0" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A458" s="0" t="s">
+        <v>906</v>
+      </c>
+      <c r="B458" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C458" s="0" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A459" s="0" t="s">
+        <v>908</v>
+      </c>
+      <c r="B459" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C459" s="0" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A460" s="0" t="s">
+        <v>910</v>
+      </c>
+      <c r="B460" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C460" s="0" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A461" s="0" t="s">
+        <v>912</v>
+      </c>
+      <c r="B461" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C461" s="0" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A462" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="B462" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C462" s="0" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A463" s="0" t="s">
+        <v>916</v>
+      </c>
+      <c r="B463" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C463" s="0" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A464" s="0" t="s">
+        <v>918</v>
+      </c>
+      <c r="B464" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C464" s="0" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A465" s="0" t="s">
+        <v>920</v>
+      </c>
+      <c r="B465" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C465" s="0" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A466" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="B466" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C466" s="0" t="s">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A467" s="0" t="s">
+        <v>924</v>
+      </c>
+      <c r="B467" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C467" s="0" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A468" s="0" t="s">
+        <v>926</v>
+      </c>
+      <c r="B468" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C468" s="0" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A469" s="0" t="s">
+        <v>928</v>
+      </c>
+      <c r="B469" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C469" s="0" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A470" s="0" t="s">
+        <v>930</v>
+      </c>
+      <c r="B470" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C470" s="0" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A471" s="0" t="s">
+        <v>932</v>
+      </c>
+      <c r="B471" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C471" s="0" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A472" s="0" t="s">
+        <v>934</v>
+      </c>
+      <c r="B472" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C472" s="0" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A473" s="0" t="s">
+        <v>936</v>
+      </c>
+      <c r="B473" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C473" s="0" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A474" s="0" t="s">
+        <v>938</v>
+      </c>
+      <c r="B474" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C474" s="0" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A475" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="B475" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C475" s="0" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A476" s="0" t="s">
+        <v>942</v>
+      </c>
+      <c r="B476" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C476" s="0" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A477" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B477" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C477" s="0" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A478" s="0" t="s">
+        <v>946</v>
+      </c>
+      <c r="B478" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C478" s="0" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A479" s="0" t="s">
+        <v>948</v>
+      </c>
+      <c r="B479" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C479" s="0" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A480" s="0" t="s">
+        <v>950</v>
+      </c>
+      <c r="B480" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C480" s="0" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A481" s="0" t="s">
+        <v>952</v>
+      </c>
+      <c r="B481" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C481" s="0" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A482" s="0" t="s">
+        <v>954</v>
+      </c>
+      <c r="B482" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C482" s="0" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A483" s="0" t="s">
+        <v>956</v>
+      </c>
+      <c r="B483" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C483" s="0" t="s">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A484" s="0" t="s">
+        <v>958</v>
+      </c>
+      <c r="B484" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C484" s="0" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A485" s="0" t="s">
+        <v>960</v>
+      </c>
+      <c r="B485" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C485" s="0" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A486" s="0" t="s">
+        <v>962</v>
+      </c>
+      <c r="B486" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C486" s="0" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A487" s="0" t="s">
+        <v>964</v>
+      </c>
+      <c r="B487" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C487" s="0" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A488" s="0" t="s">
+        <v>966</v>
+      </c>
+      <c r="B488" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C488" s="0" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A489" s="0" t="s">
+        <v>968</v>
+      </c>
+      <c r="B489" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C489" s="0" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A490" s="0" t="s">
+        <v>970</v>
+      </c>
+      <c r="B490" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C490" s="0" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A491" s="0" t="s">
+        <v>972</v>
+      </c>
+      <c r="B491" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C491" s="0" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A492" s="0" t="s">
+        <v>974</v>
+      </c>
+      <c r="B492" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C492" s="0" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A493" s="0" t="s">
+        <v>976</v>
+      </c>
+      <c r="B493" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C493" s="0" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A494" s="0" t="s">
+        <v>978</v>
+      </c>
+      <c r="B494" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C494" s="0" t="s">
+        <v>979</v>
+      </c>
+    </row>
+    <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A495" s="0" t="s">
+        <v>980</v>
+      </c>
+      <c r="B495" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C495" s="0" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A496" s="0" t="s">
+        <v>982</v>
+      </c>
+      <c r="B496" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C496" s="0" t="s">
+        <v>983</v>
+      </c>
+      <c r="D496" s="0" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A497" s="0" t="s">
+        <v>985</v>
+      </c>
+      <c r="B497" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C497" s="0" t="s">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A498" s="0" t="s">
+        <v>987</v>
+      </c>
+      <c r="B498" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C498" s="0" t="s">
+        <v>988</v>
+      </c>
+    </row>
+    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A499" s="0" t="s">
+        <v>989</v>
+      </c>
+      <c r="B499" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C499" s="0" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A500" s="0" t="s">
+        <v>991</v>
+      </c>
+      <c r="B500" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C500" s="0" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A501" s="0" t="s">
+        <v>993</v>
+      </c>
+      <c r="B501" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C501" s="0" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A502" s="0" t="s">
+        <v>995</v>
+      </c>
+      <c r="B502" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C502" s="0" t="s">
+        <v>577</v>
+      </c>
+      <c r="D502" s="0" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A503" s="0" t="s">
+        <v>997</v>
+      </c>
+      <c r="B503" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C503" s="0" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A504" s="0" t="s">
+        <v>999</v>
+      </c>
+      <c r="B504" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C504" s="0" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A505" s="0" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B505" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C505" s="0" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A506" s="0" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B506" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C506" s="0" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A507" s="0" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B507" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C507" s="0" t="s">
+        <v>1006</v>
+      </c>
+      <c r="D507" s="0" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A508" s="3" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B508" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C508" s="0" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D508" s="0" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A509" s="0" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B509" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C509" s="0" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D509" s="0" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A510" s="0" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B510" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C510" s="0" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D510" s="0" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A511" s="0" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B511" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C511" s="0" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A512" s="0" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B512" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C512" s="0" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D512" s="0" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A513" s="0" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B513" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C513" s="0" t="s">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A514" s="0" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B514" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C514" s="0" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A515" s="0" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B515" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C515" s="0" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A516" s="0" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B516" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C516" s="0" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A517" s="0" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B517" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C517" s="0" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D517" s="0" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A518" s="0" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B518" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C518" s="0" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A519" s="0" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B519" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C519" s="0" t="s">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A520" s="0" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B520" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C520" s="0" t="s">
+        <v>1038</v>
+      </c>
+      <c r="D520" s="0" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A521" s="0" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B521" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C521" s="0" t="s">
+        <v>1041</v>
+      </c>
+      <c r="D521" s="0" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A522" s="0" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B522" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C522" s="0" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A523" s="0" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B523" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C523" s="0" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A524" s="0" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B524" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C524" s="0" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A525" s="0" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B525" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C525" s="0" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A526" s="0" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B526" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C526" s="0" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A527" s="0" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B527" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C527" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A528" s="0" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B528" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C528" s="0" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A529" s="0" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B529" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C529" s="0" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A530" s="0" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B530" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C530" s="0" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A531" s="0" t="s">
+        <v>1059</v>
+      </c>
+      <c r="B531" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C531" s="0" t="s">
+        <v>571</v>
+      </c>
+      <c r="D531" s="0" t="s">
+        <v>1060</v>
       </c>
     </row>
   </sheetData>

</xml_diff>